<commit_message>
Roughly calibrated power sector variables to align with EU ETS scenario from BNEF.
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\CSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\European Union\Models\eps-eu\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E686583-1FEC-4314-9011-6556A4E44EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31F40D1-0B86-4323-BA0F-17D9FF97A89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="29355" yWindow="4050" windowWidth="24825" windowHeight="15930" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t xml:space="preserve">Source: </t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>CSC Capacity Supply Curve Share of Cost Effective Capacity Built in a Single Year</t>
+  </si>
+  <si>
+    <t>For the EU, we have loosely calibrated against the EU outlook from BNEF.</t>
   </si>
 </sst>
 </file>
@@ -501,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3D2DEE-686E-48A0-AC3D-0F54DEA5D0EC}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,6 +538,11 @@
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -547,10 +555,10 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B1" sqref="B1:P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,97 +566,103 @@
     <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1">
-        <v>0</v>
+      <c r="B1" t="s">
+        <v>3</v>
       </c>
       <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
         <v>0.25</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>0.5</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>0.75</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <v>1</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <v>1.25</v>
       </c>
-      <c r="H1">
+      <c r="I1">
         <v>1.5</v>
       </c>
-      <c r="I1">
+      <c r="J1">
         <v>1.75</v>
       </c>
-      <c r="J1">
+      <c r="K1">
         <v>2</v>
       </c>
-      <c r="K1">
+      <c r="L1">
         <v>2.25</v>
       </c>
-      <c r="L1">
+      <c r="M1">
         <v>2.5</v>
       </c>
-      <c r="M1">
+      <c r="N1">
         <v>2.75</v>
       </c>
-      <c r="N1">
+      <c r="O1">
         <v>3</v>
       </c>
-      <c r="O1">
+      <c r="P1">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>1.1000000000000001</v>
-      </c>
       <c r="D2">
-        <v>1.3</v>
+        <v>1.369170386</v>
       </c>
       <c r="E2">
-        <v>1.6</v>
+        <v>1.74616726</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>2.2269690689999999</v>
       </c>
       <c r="G2">
-        <v>2.5</v>
+        <v>2.8401581839999999</v>
       </c>
       <c r="H2">
-        <v>3.1</v>
+        <v>3.6221870429999998</v>
       </c>
       <c r="I2">
-        <v>3.8</v>
+        <v>4.619545156</v>
       </c>
       <c r="J2">
-        <v>4.5999999999999996</v>
+        <v>5.8915227699999999</v>
       </c>
       <c r="K2">
-        <v>5.5</v>
+        <v>7.5137355259999996</v>
       </c>
       <c r="L2">
-        <v>6.5</v>
+        <v>9.5826195980000008</v>
       </c>
       <c r="M2">
-        <v>7.6</v>
+        <v>12.22116456</v>
       </c>
       <c r="N2">
-        <v>8.8000000000000007</v>
+        <v>15.586224809999999</v>
       </c>
       <c r="O2">
+        <v>19.87784409</v>
+      </c>
+      <c r="P2">
         <v>1000</v>
       </c>
     </row>
@@ -698,8 +712,8 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="AF8" sqref="AF8:AG8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:AE25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,94 +1296,94 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="C7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="D7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="E7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="F7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="G7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="H7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="I7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="J7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="K7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="L7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="M7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="N7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="O7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="P7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="Q7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="R7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="S7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="T7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="U7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="V7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="W7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="X7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="Y7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="Z7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="AA7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="AB7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="AC7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="AD7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="AE7">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Increase capacity supply curve for NG CC & peaker plants to fixcapacity building bug in policy scenarios
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\European Union\Models\eps-eu\InputData\elec\CSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7358C4-500D-4E1E-8548-A109AEB9316D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F42B4E-3B19-40AA-A265-B06A582ABFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="62880" yWindow="1635" windowWidth="23295" windowHeight="15465" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2470,31 +2470,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3D2DEE-686E-48A0-AC3D-0F54DEA5D0EC}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="88.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2502,17 +2502,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>1.45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -2553,12 +2553,12 @@
       <selection activeCell="B1" sqref="B1:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2682,17 +2682,17 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2712,16 +2712,16 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:AE13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3006,102 +3006,102 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="M4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="N4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="O4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="P4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="Q4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="R4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="S4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="T4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="U4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="V4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="W4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="X4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="Y4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="Z4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="AA4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="AB4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="AC4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="AD4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="AE4">
-        <v>0.23</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3386,7 +3386,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -3861,102 +3861,102 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="B13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="J13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="K13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="L13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="M13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="N13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="O13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="P13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="Q13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="R13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="S13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="T13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="U13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="V13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="W13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="X13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="Y13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="Z13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="AA13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="AB13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="AC13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="AD13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="AE13">
-        <v>0.23</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -4621,7 +4621,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -4716,7 +4716,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -4811,7 +4811,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -4906,7 +4906,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Modifies calibration parameters for renewable projections
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D5C1E8-53DC-4FDB-A6B0-246D062C8359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABD8BD6-4B47-4AAD-A7FE-0385A8BBB978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="16270" windowHeight="10800" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1698,7 +1698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3D2DEE-686E-48A0-AC3D-0F54DEA5D0EC}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -1777,8 +1777,8 @@
   </sheetPr>
   <dimension ref="A1:AU2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2163,8 +2163,8 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:AE8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:AE8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2747,94 +2747,94 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="C7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="D7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="E7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="F7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="G7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="H7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="I7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="J7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="K7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="L7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="M7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="N7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="O7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="P7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="Q7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="R7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="S7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="T7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="U7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="V7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="W7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="X7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="Y7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="Z7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="AA7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="AB7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="AC7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="AD7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="AE7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.35">
@@ -2842,94 +2842,94 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="C8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="D8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="E8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="F8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="G8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="H8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="I8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="J8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="K8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="L8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="M8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="N8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="O8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="P8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="Q8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="R8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="S8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="T8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="U8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="V8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="W8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="X8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="Y8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="Z8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="AA8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="AB8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="AC8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="AD8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="AE8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
pulls most recent US EPS commit
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\CSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C110F7-550A-49C7-9993-BC93998675E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0D785E-3678-4517-A5F6-3A839C381C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2470,31 +2470,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3D2DEE-686E-48A0-AC3D-0F54DEA5D0EC}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="88.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2502,17 +2502,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>1.45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -2553,12 +2553,12 @@
       <selection activeCell="B1" sqref="B1:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2682,17 +2682,17 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2712,16 +2712,16 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AE25"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:AE7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3291,102 +3291,102 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="C7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="F7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="G7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="H7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="I7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="J7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="K7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="L7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="M7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="N7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="O7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="P7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="Q7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="R7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="S7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="T7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="U7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="V7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="W7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="X7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="Y7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="Z7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="AA7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="AB7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="AC7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="AD7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="AE7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -4621,7 +4621,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -4716,7 +4716,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -4811,7 +4811,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -4906,7 +4906,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>30</v>
       </c>

</xml_diff>